<commit_message>
Update: Excel - Chart File
</commit_message>
<xml_diff>
--- a/notes/excel/charts.xlsx
+++ b/notes/excel/charts.xlsx
@@ -1,21 +1,158 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/github/analytics-portfolio/notes/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA04C7DD-8BCF-4FE5-B548-55CBD210AC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB011859-1F07-BA4C-8F52-575CDAC00470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03CEABDE-3C67-4836-9FDD-609F2D7E7F08}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{03CEABDE-3C67-4836-9FDD-609F2D7E7F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="3" r:id="rId1"/>
     <sheet name="Chart Sheet" sheetId="4" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sales!$A$3</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sales!$A$4</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sales!$B$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.100" hidden="1">Sales!$B$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.101" hidden="1">Sales!$B$6:$M$6</definedName>
+    <definedName name="_xlchart.v1.102" hidden="1">Sales!$B$7:$M$7</definedName>
+    <definedName name="_xlchart.v1.103" hidden="1">Sales!$B$8:$M$8</definedName>
+    <definedName name="_xlchart.v1.104" hidden="1">Sales!$B$9:$M$9</definedName>
+    <definedName name="_xlchart.v1.105" hidden="1">Sales!$A$3</definedName>
+    <definedName name="_xlchart.v1.106" hidden="1">Sales!$A$4</definedName>
+    <definedName name="_xlchart.v1.107" hidden="1">Sales!$A$5</definedName>
+    <definedName name="_xlchart.v1.108" hidden="1">Sales!$A$6</definedName>
+    <definedName name="_xlchart.v1.109" hidden="1">Sales!$A$7</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sales!$B$6:$M$6</definedName>
+    <definedName name="_xlchart.v1.110" hidden="1">Sales!$A$8</definedName>
+    <definedName name="_xlchart.v1.111" hidden="1">Sales!$A$9</definedName>
+    <definedName name="_xlchart.v1.112" hidden="1">Sales!$B$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.113" hidden="1">Sales!$B$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.114" hidden="1">Sales!$B$4:$M$4</definedName>
+    <definedName name="_xlchart.v1.115" hidden="1">Sales!$B$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.116" hidden="1">Sales!$B$6:$M$6</definedName>
+    <definedName name="_xlchart.v1.117" hidden="1">Sales!$B$7:$M$7</definedName>
+    <definedName name="_xlchart.v1.118" hidden="1">Sales!$B$8:$M$8</definedName>
+    <definedName name="_xlchart.v1.119" hidden="1">Sales!$B$9:$M$9</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sales!$B$7:$M$7</definedName>
+    <definedName name="_xlchart.v1.120" hidden="1">Sales!$A$3</definedName>
+    <definedName name="_xlchart.v1.121" hidden="1">Sales!$A$4</definedName>
+    <definedName name="_xlchart.v1.122" hidden="1">Sales!$A$5</definedName>
+    <definedName name="_xlchart.v1.123" hidden="1">Sales!$A$6</definedName>
+    <definedName name="_xlchart.v1.124" hidden="1">Sales!$A$7</definedName>
+    <definedName name="_xlchart.v1.125" hidden="1">Sales!$A$8</definedName>
+    <definedName name="_xlchart.v1.126" hidden="1">Sales!$A$9</definedName>
+    <definedName name="_xlchart.v1.127" hidden="1">Sales!$B$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.128" hidden="1">Sales!$B$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.129" hidden="1">Sales!$B$4:$M$4</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sales!$B$8:$M$8</definedName>
+    <definedName name="_xlchart.v1.130" hidden="1">Sales!$B$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.131" hidden="1">Sales!$B$6:$M$6</definedName>
+    <definedName name="_xlchart.v1.132" hidden="1">Sales!$B$7:$M$7</definedName>
+    <definedName name="_xlchart.v1.133" hidden="1">Sales!$B$8:$M$8</definedName>
+    <definedName name="_xlchart.v1.134" hidden="1">Sales!$B$9:$M$9</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sales!$B$9:$M$9</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sales!$A$3</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sales!$A$4</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sales!$A$5</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sales!$A$6</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sales!$A$7</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sales!$A$5</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sales!$A$8</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sales!$A$9</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sales!$B$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sales!$B$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sales!$B$4:$M$4</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sales!$B$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sales!$B$6:$M$6</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sales!$B$7:$M$7</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sales!$B$8:$M$8</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sales!$B$9:$M$9</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sales!$A$6</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Sales!$A$3</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Sales!$A$4</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Sales!$A$5</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Sales!$A$6</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Sales!$A$7</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Sales!$A$8</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Sales!$A$9</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Sales!$B$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Sales!$B$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Sales!$B$4:$M$4</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sales!$A$7</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Sales!$B$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Sales!$B$6:$M$6</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Sales!$B$7:$M$7</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">Sales!$B$8:$M$8</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">Sales!$B$9:$M$9</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">Sales!$A$3</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">Sales!$A$4</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">Sales!$A$5</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">Sales!$A$6</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">Sales!$A$7</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sales!$A$8</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">Sales!$A$8</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">Sales!$A$9</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">Sales!$B$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">Sales!$B$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">Sales!$B$4:$M$4</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">Sales!$B$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">Sales!$B$6:$M$6</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">Sales!$B$7:$M$7</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">Sales!$B$8:$M$8</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">Sales!$B$9:$M$9</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sales!$A$9</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">Sales!$A$3</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">Sales!$A$4</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">Sales!$A$5</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">Sales!$A$6</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">Sales!$A$7</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">Sales!$A$8</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">Sales!$A$9</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">Sales!$B$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">Sales!$B$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">Sales!$B$4:$M$4</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sales!$B$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">Sales!$B$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">Sales!$B$6:$M$6</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">Sales!$B$7:$M$7</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">Sales!$B$8:$M$8</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">Sales!$B$9:$M$9</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">Sales!$A$3</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">Sales!$A$4</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">Sales!$A$5</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">Sales!$A$6</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">Sales!$A$7</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sales!$B$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.80" hidden="1">Sales!$A$8</definedName>
+    <definedName name="_xlchart.v1.81" hidden="1">Sales!$A$9</definedName>
+    <definedName name="_xlchart.v1.82" hidden="1">Sales!$B$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.83" hidden="1">Sales!$B$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.84" hidden="1">Sales!$B$4:$M$4</definedName>
+    <definedName name="_xlchart.v1.85" hidden="1">Sales!$B$5:$M$5</definedName>
+    <definedName name="_xlchart.v1.86" hidden="1">Sales!$B$6:$M$6</definedName>
+    <definedName name="_xlchart.v1.87" hidden="1">Sales!$B$7:$M$7</definedName>
+    <definedName name="_xlchart.v1.88" hidden="1">Sales!$B$8:$M$8</definedName>
+    <definedName name="_xlchart.v1.89" hidden="1">Sales!$B$9:$M$9</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sales!$B$4:$M$4</definedName>
+    <definedName name="_xlchart.v1.90" hidden="1">Sales!$A$3</definedName>
+    <definedName name="_xlchart.v1.91" hidden="1">Sales!$A$4</definedName>
+    <definedName name="_xlchart.v1.92" hidden="1">Sales!$A$5</definedName>
+    <definedName name="_xlchart.v1.93" hidden="1">Sales!$A$6</definedName>
+    <definedName name="_xlchart.v1.94" hidden="1">Sales!$A$7</definedName>
+    <definedName name="_xlchart.v1.95" hidden="1">Sales!$A$8</definedName>
+    <definedName name="_xlchart.v1.96" hidden="1">Sales!$A$9</definedName>
+    <definedName name="_xlchart.v1.97" hidden="1">Sales!$B$2:$M$2</definedName>
+    <definedName name="_xlchart.v1.98" hidden="1">Sales!$B$3:$M$3</definedName>
+    <definedName name="_xlchart.v1.99" hidden="1">Sales!$B$4:$M$4</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -124,7 +261,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +271,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,13 +293,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,6 +316,1532 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Products</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Sold per Month</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.1280959303769595E-2"/>
+          <c:y val="1.8552871178552879E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-KW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$3:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C61B-3E41-94B6-8458702F2DE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$5:$M$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C61B-3E41-94B6-8458702F2DE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$7:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>103</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C61B-3E41-94B6-8458702F2DE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2032754207"/>
+        <c:axId val="2032756831"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2032754207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2032756831"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2032756831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Amount</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-KW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2032754207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-KW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-KW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>42544</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>106681</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{215DAC17-53E0-0005-0E20-EE9B8565784F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="470642" cy="264431"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14982868-BCCA-21E0-8B6E-CB601BFB2694}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6845300" y="2768600"/>
+          <a:ext cx="470642" cy="264431"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>5071</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="470642" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B5D16A-208F-1592-C9BA-BAFC67C5EEE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6845300" y="3238500"/>
+          <a:ext cx="470642" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>1583</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116440</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="399148" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECA70B6F-8034-F516-92DA-224673F80350}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6845300" y="3545440"/>
+          <a:ext cx="399148" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>811</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>75458</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6350741" cy="530530"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BD3786B-DDD1-C4B6-906F-0A53C9625D59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="75458" y="50800"/>
+          <a:ext cx="6350741" cy="530530"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0"/>
+            <a:t>Paper,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" baseline="0"/>
+            <a:t> Manila Folder, and 3 Ring Binder are the top three products sold for the year. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Allocating budget for distribution and marketing can increase our revenue.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,17 +2143,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41930B34-5114-49CB-81BC-662EB848F545}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -501,7 +2171,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -542,7 +2212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -587,7 +2257,7 @@
         <v>5071</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -632,7 +2302,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -677,7 +2347,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -722,7 +2392,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -767,7 +2437,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -812,7 +2482,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -857,7 +2527,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -910,7 +2580,7 @@
         <v>721</v>
       </c>
       <c r="N10" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(N3:N9)</f>
         <v>9077</v>
       </c>
     </row>
@@ -927,12 +2597,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B444C6-5638-496B-93B2-259D582C3A1D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="4"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>